<commit_message>
removed unnecessary  code snippets
</commit_message>
<xml_diff>
--- a/data/religions.xlsx
+++ b/data/religions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mario/Resilio Sync/application-files/webstorm/ivis__projekt-2018/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Programming_Workspace\ivis\ivis_religious_denominations_in_switzerland\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8E9A98-6746-7941-B69A-A2ABF5799023}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16980" xr2:uid="{B3086ECD-E67C-4A48-BF44-F19BFCA864EC}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="28800" windowHeight="16980"/>
   </bookViews>
   <sheets>
     <sheet name="religionen 2011-2016" sheetId="1" r:id="rId1"/>
@@ -141,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -157,12 +156,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -178,14 +183,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{4BD35CA4-B842-FC47-BC2C-84138FA8A2C9}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -496,20 +504,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA5C2F9-39FD-6041-ABE6-75B9D48C6681}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="9" max="9" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -541,39 +549,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>2011</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>6587556</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>1830143</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>2532217</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>368698</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="4">
         <v>16763</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
         <v>320958</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="4">
         <v>80758</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>1356795</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -605,7 +613,7 @@
         <v>152501</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -637,7 +645,7 @@
         <v>29087</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -669,7 +677,7 @@
         <v>124823</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -701,7 +709,7 @@
         <v>124502</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -733,7 +741,7 @@
         <v>30218</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -765,7 +773,7 @@
         <v>53835</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -797,7 +805,7 @@
         <v>54118</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -829,7 +837,7 @@
         <v>6497</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -861,7 +869,7 @@
         <v>67340</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -893,7 +901,7 @@
         <v>56579</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -925,7 +933,7 @@
         <v>112256</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -957,7 +965,7 @@
         <v>270765</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -989,7 +997,7 @@
         <v>5332</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1021,7 +1029,7 @@
         <v>13579</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +1061,7 @@
         <v>7202</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1085,7 +1093,7 @@
         <v>873.64601000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1117,7 +1125,7 @@
         <v>59874</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>21796</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1181,7 +1189,7 @@
         <v>34704</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1213,7 +1221,7 @@
         <v>42625</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -1245,7 +1253,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1277,7 +1285,7 @@
         <v>16101</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
@@ -1309,7 +1317,7 @@
         <v>3046</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -1341,7 +1349,7 @@
         <v>4817</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
@@ -1373,7 +1381,7 @@
         <v>17388</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -1405,39 +1413,39 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="4">
         <v>2012</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="4">
         <v>6662333</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="4">
         <v>1792064</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="4">
         <v>2544602</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="4">
         <v>378512</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="4">
         <v>16889</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="4">
         <v>328011</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="4">
         <v>88719</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="4">
         <v>1428403</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -1469,7 +1477,7 @@
         <v>160477</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1501,7 +1509,7 @@
         <v>29647</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
@@ -1533,7 +1541,7 @@
         <v>126951</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1565,7 +1573,7 @@
         <v>135348</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1597,7 +1605,7 @@
         <v>33627</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
@@ -1629,7 +1637,7 @@
         <v>58110</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>17</v>
       </c>
@@ -1661,7 +1669,7 @@
         <v>56360</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>18</v>
       </c>
@@ -1693,7 +1701,7 @@
         <v>7054</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1725,7 +1733,7 @@
         <v>69828</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
@@ -1757,7 +1765,7 @@
         <v>59970</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>21</v>
       </c>
@@ -1789,7 +1797,7 @@
         <v>118299</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
@@ -1821,7 +1829,7 @@
         <v>284207</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>23</v>
       </c>
@@ -1853,7 +1861,7 @@
         <v>4972</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>24</v>
       </c>
@@ -1885,7 +1893,7 @@
         <v>14789</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>25</v>
       </c>
@@ -1917,7 +1925,7 @@
         <v>7204</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>26</v>
       </c>
@@ -1949,7 +1957,7 @@
         <v>932.47335999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1989,7 @@
         <v>61116</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>28</v>
       </c>
@@ -2013,7 +2021,7 @@
         <v>23003</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>29</v>
       </c>
@@ -2045,7 +2053,7 @@
         <v>36193</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
@@ -2077,7 +2085,7 @@
         <v>44096</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
@@ -2109,7 +2117,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>32</v>
       </c>
@@ -2141,7 +2149,7 @@
         <v>17965</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>33</v>
       </c>
@@ -2173,7 +2181,7 @@
         <v>3616</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
@@ -2205,7 +2213,7 @@
         <v>4914</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>35</v>
       </c>
@@ -2237,7 +2245,7 @@
         <v>18974</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>36</v>
       </c>
@@ -2269,39 +2277,39 @@
         <v>48377</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="4">
         <v>2013</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="4">
         <v>6744794</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="4">
         <v>1762892</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="4">
         <v>2562396</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56" s="4">
         <v>389608</v>
       </c>
-      <c r="G56" s="1">
+      <c r="G56" s="4">
         <v>16830</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H56" s="4">
         <v>341572</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I56" s="4">
         <v>89259</v>
       </c>
-      <c r="J56" s="1">
+      <c r="J56" s="4">
         <v>1497521</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>11</v>
       </c>
@@ -2333,7 +2341,7 @@
         <v>169929</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>12</v>
       </c>
@@ -2365,7 +2373,7 @@
         <v>31712</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>13</v>
       </c>
@@ -2397,7 +2405,7 @@
         <v>133642</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>14</v>
       </c>
@@ -2429,7 +2437,7 @@
         <v>142122</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>15</v>
       </c>
@@ -2461,7 +2469,7 @@
         <v>35969</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>16</v>
       </c>
@@ -2493,7 +2501,7 @@
         <v>60209</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>17</v>
       </c>
@@ -2525,7 +2533,7 @@
         <v>58329</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>18</v>
       </c>
@@ -2557,7 +2565,7 @@
         <v>7556</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>19</v>
       </c>
@@ -2589,7 +2597,7 @@
         <v>72719</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -2621,7 +2629,7 @@
         <v>59710</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>21</v>
       </c>
@@ -2653,7 +2661,7 @@
         <v>125195</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>22</v>
       </c>
@@ -2685,7 +2693,7 @@
         <v>296724</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>23</v>
       </c>
@@ -2717,7 +2725,7 @@
         <v>5230</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>24</v>
       </c>
@@ -2749,7 +2757,7 @@
         <v>14940</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>25</v>
       </c>
@@ -2781,7 +2789,7 @@
         <v>8209</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>26</v>
       </c>
@@ -2813,7 +2821,7 @@
         <v>828.56652999999994</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>27</v>
       </c>
@@ -2845,7 +2853,7 @@
         <v>62978</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>28</v>
       </c>
@@ -2877,7 +2885,7 @@
         <v>24380</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>29</v>
       </c>
@@ -2909,7 +2917,7 @@
         <v>38569</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -2941,7 +2949,7 @@
         <v>50151</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>31</v>
       </c>
@@ -2973,7 +2981,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>32</v>
       </c>
@@ -3005,7 +3013,7 @@
         <v>17867</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>33</v>
       </c>
@@ -3037,7 +3045,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -3069,7 +3077,7 @@
         <v>4758</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>35</v>
       </c>
@@ -3101,7 +3109,7 @@
         <v>19690</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>36</v>
       </c>
@@ -3133,39 +3141,39 @@
         <v>50296</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+    <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="4">
         <v>2014</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" s="4">
         <v>6829610</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83" s="4">
         <v>1742823</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="4">
         <v>2585788</v>
       </c>
-      <c r="F83" s="1">
+      <c r="F83" s="4">
         <v>392070</v>
       </c>
-      <c r="G83" s="1">
+      <c r="G83" s="4">
         <v>15893</v>
       </c>
-      <c r="H83" s="1">
+      <c r="H83" s="4">
         <v>346208</v>
       </c>
-      <c r="I83" s="1">
+      <c r="I83" s="4">
         <v>90469</v>
       </c>
-      <c r="J83" s="1">
+      <c r="J83" s="4">
         <v>1572027</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>11</v>
       </c>
@@ -3197,7 +3205,7 @@
         <v>175774</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>12</v>
       </c>
@@ -3229,7 +3237,7 @@
         <v>34352</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>13</v>
       </c>
@@ -3261,7 +3269,7 @@
         <v>134063</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>14</v>
       </c>
@@ -3293,7 +3301,7 @@
         <v>151665</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>15</v>
       </c>
@@ -3325,7 +3333,7 @@
         <v>38365</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>16</v>
       </c>
@@ -3357,7 +3365,7 @@
         <v>62660</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>17</v>
       </c>
@@ -3389,7 +3397,7 @@
         <v>61095</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>18</v>
       </c>
@@ -3421,7 +3429,7 @@
         <v>7432</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>19</v>
       </c>
@@ -3453,7 +3461,7 @@
         <v>73591</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>20</v>
       </c>
@@ -3485,7 +3493,7 @@
         <v>65610</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>21</v>
       </c>
@@ -3517,7 +3525,7 @@
         <v>133778</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>22</v>
       </c>
@@ -3549,7 +3557,7 @@
         <v>310429</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>23</v>
       </c>
@@ -3581,7 +3589,7 @@
         <v>6306</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>24</v>
       </c>
@@ -3613,7 +3621,7 @@
         <v>15378</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>25</v>
       </c>
@@ -3645,7 +3653,7 @@
         <v>7755</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>26</v>
       </c>
@@ -3677,7 +3685,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>27</v>
       </c>
@@ -3709,7 +3717,7 @@
         <v>67350</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>28</v>
       </c>
@@ -3741,7 +3749,7 @@
         <v>26377</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>29</v>
       </c>
@@ -3773,7 +3781,7 @@
         <v>41488</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>30</v>
       </c>
@@ -3805,7 +3813,7 @@
         <v>51567</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>31</v>
       </c>
@@ -3837,7 +3845,7 @@
         <v>2951</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>32</v>
       </c>
@@ -3869,7 +3877,7 @@
         <v>21037</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>33</v>
       </c>
@@ -3901,7 +3909,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>34</v>
       </c>
@@ -3933,7 +3941,7 @@
         <v>6095</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>35</v>
       </c>
@@ -3965,7 +3973,7 @@
         <v>20420</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>36</v>
       </c>
@@ -3997,39 +4005,39 @@
         <v>51710</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="4">
         <v>2015</v>
       </c>
-      <c r="C110" s="1">
+      <c r="C110" s="4">
         <v>6907818</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110" s="4">
         <v>1722222</v>
       </c>
-      <c r="E110" s="1">
+      <c r="E110" s="4">
         <v>2573443</v>
       </c>
-      <c r="F110" s="1">
+      <c r="F110" s="4">
         <v>403429</v>
       </c>
-      <c r="G110" s="1">
+      <c r="G110" s="4">
         <v>17250</v>
       </c>
-      <c r="H110" s="1">
+      <c r="H110" s="4">
         <v>351961</v>
       </c>
-      <c r="I110" s="1">
+      <c r="I110" s="4">
         <v>93396</v>
       </c>
-      <c r="J110" s="1">
+      <c r="J110" s="4">
         <v>1653568</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>11</v>
       </c>
@@ -4061,7 +4069,7 @@
         <v>190691</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>12</v>
       </c>
@@ -4093,7 +4101,7 @@
         <v>35745</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>13</v>
       </c>
@@ -4125,7 +4133,7 @@
         <v>143699</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>14</v>
       </c>
@@ -4157,7 +4165,7 @@
         <v>158270</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>15</v>
       </c>
@@ -4189,7 +4197,7 @@
         <v>41158</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>16</v>
       </c>
@@ -4221,7 +4229,7 @@
         <v>64566</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>17</v>
       </c>
@@ -4253,7 +4261,7 @@
         <v>62261</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>18</v>
       </c>
@@ -4285,7 +4293,7 @@
         <v>8732</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>19</v>
       </c>
@@ -4317,7 +4325,7 @@
         <v>74825</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>20</v>
       </c>
@@ -4349,7 +4357,7 @@
         <v>68312</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>21</v>
       </c>
@@ -4381,7 +4389,7 @@
         <v>143428</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>22</v>
       </c>
@@ -4413,7 +4421,7 @@
         <v>328713</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>23</v>
       </c>
@@ -4445,7 +4453,7 @@
         <v>5957</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>24</v>
       </c>
@@ -4477,7 +4485,7 @@
         <v>15552</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>25</v>
       </c>
@@ -4509,7 +4517,7 @@
         <v>8423</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>26</v>
       </c>
@@ -4541,7 +4549,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>27</v>
       </c>
@@ -4573,7 +4581,7 @@
         <v>71183</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>28</v>
       </c>
@@ -4605,7 +4613,7 @@
         <v>24324</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>29</v>
       </c>
@@ -4637,7 +4645,7 @@
         <v>42803</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>30</v>
       </c>
@@ -4669,7 +4677,7 @@
         <v>54229</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>31</v>
       </c>
@@ -4701,7 +4709,7 @@
         <v>2917</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>32</v>
       </c>
@@ -4733,7 +4741,7 @@
         <v>22012</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>33</v>
       </c>
@@ -4765,7 +4773,7 @@
         <v>3886</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>34</v>
       </c>
@@ -4797,7 +4805,7 @@
         <v>5630</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>35</v>
       </c>
@@ -4829,7 +4837,7 @@
         <v>22104</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>36</v>
       </c>
@@ -4861,39 +4869,39 @@
         <v>53057</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
+    <row r="137" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="4">
         <v>2016</v>
       </c>
-      <c r="C137" s="1">
+      <c r="C137" s="4">
         <v>6981380.9999999302</v>
       </c>
-      <c r="D137" s="1">
+      <c r="D137" s="4">
         <v>1713116.72818507</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137" s="4">
         <v>2550646.5747465999</v>
       </c>
-      <c r="F137" s="1">
+      <c r="F137" s="4">
         <v>410164.71618767601</v>
       </c>
-      <c r="G137" s="1">
+      <c r="G137" s="4">
         <v>17731.656500756701</v>
       </c>
-      <c r="H137" s="1">
+      <c r="H137" s="4">
         <v>362973.41586231301</v>
       </c>
-      <c r="I137" s="1">
+      <c r="I137" s="4">
         <v>96354.392855077604</v>
       </c>
-      <c r="J137" s="1">
+      <c r="J137" s="4">
         <v>1740916.5161851901</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>11</v>
       </c>
@@ -4925,7 +4933,7 @@
         <v>198852.07086324101</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>12</v>
       </c>
@@ -4957,7 +4965,7 @@
         <v>39286.471767380499</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>13</v>
       </c>
@@ -4989,7 +4997,7 @@
         <v>151693.66559743701</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>14</v>
       </c>
@@ -5021,7 +5029,7 @@
         <v>168953.15633999801</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>15</v>
       </c>
@@ -5053,7 +5061,7 @@
         <v>42616.413113732102</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>16</v>
       </c>
@@ -5085,7 +5093,7 @@
         <v>69771.327424785399</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>17</v>
       </c>
@@ -5117,7 +5125,7 @@
         <v>65447.699883351503</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>18</v>
       </c>
@@ -5149,7 +5157,7 @@
         <v>8807.0101925609997</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>19</v>
       </c>
@@ -5181,7 +5189,7 @@
         <v>77321.307175027701</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
         <v>20</v>
       </c>
@@ -5213,7 +5221,7 @@
         <v>69684.096558527104</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>21</v>
       </c>
@@ -5245,7 +5253,7 @@
         <v>145897.37864216801</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>22</v>
       </c>
@@ -5277,7 +5285,7 @@
         <v>340852.10092930502</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
         <v>23</v>
       </c>
@@ -5309,7 +5317,7 @@
         <v>7168.69617519844</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>24</v>
       </c>
@@ -5341,7 +5349,7 @@
         <v>17082.587119284599</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
         <v>25</v>
       </c>
@@ -5373,7 +5381,7 @@
         <v>9634.0595574468407</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
         <v>26</v>
       </c>
@@ -5405,7 +5413,7 @@
         <v>1189.3325193016699</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
         <v>27</v>
       </c>
@@ -5437,7 +5445,7 @@
         <v>74587.011503593603</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
         <v>28</v>
       </c>
@@ -5469,7 +5477,7 @@
         <v>27659.074949431601</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
         <v>29</v>
       </c>
@@ -5501,7 +5509,7 @@
         <v>48175.351028462297</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
         <v>30</v>
       </c>
@@ -5533,7 +5541,7 @@
         <v>55887.248586481997</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
         <v>31</v>
       </c>
@@ -5565,7 +5573,7 @@
         <v>2912.1074638851901</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
         <v>32</v>
       </c>
@@ -5597,7 +5605,7 @@
         <v>24893.387150737399</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
         <v>33</v>
       </c>
@@ -5629,7 +5637,7 @@
         <v>4220.1649579956002</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>34</v>
       </c>
@@ -5661,7 +5669,7 @@
         <v>6304.4066194142697</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>35</v>
       </c>
@@ -5693,7 +5701,7 @@
         <v>22942.093096056102</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
added iso attribute to religions.csv
</commit_message>
<xml_diff>
--- a/data/religions.xlsx
+++ b/data/religions.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="religionen 2011-2016" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="65">
   <si>
     <t>kanton</t>
   </si>
@@ -135,6 +135,90 @@
   </si>
   <si>
     <t>Tessin</t>
+  </si>
+  <si>
+    <t>iso</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>VD</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>JU</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>ZH</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>UR</t>
+  </si>
+  <si>
+    <t>SZ</t>
+  </si>
+  <si>
+    <t>OW</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>ZG</t>
+  </si>
+  <si>
+    <t>TI</t>
   </si>
 </sst>
 </file>
@@ -505,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J163"/>
+  <dimension ref="A1:K163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="K137" sqref="K137:K163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -517,7 +601,7 @@
     <col min="9" max="9" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,8 +632,11 @@
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -580,8 +667,11 @@
       <c r="J2" s="4">
         <v>1356795</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -612,8 +702,11 @@
       <c r="J3" s="1">
         <v>152501</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -644,8 +737,11 @@
       <c r="J4" s="1">
         <v>29087</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -676,8 +772,11 @@
       <c r="J5" s="1">
         <v>124823</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -708,8 +807,11 @@
       <c r="J6" s="1">
         <v>124502</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -740,8 +842,11 @@
       <c r="J7" s="1">
         <v>30218</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -772,8 +877,11 @@
       <c r="J8" s="1">
         <v>53835</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -804,8 +912,11 @@
       <c r="J9" s="1">
         <v>54118</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -836,8 +947,11 @@
       <c r="J10" s="1">
         <v>6497</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -868,8 +982,11 @@
       <c r="J11" s="1">
         <v>67340</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -900,8 +1017,11 @@
       <c r="J12" s="1">
         <v>56579</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -932,8 +1052,11 @@
       <c r="J13" s="1">
         <v>112256</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -964,8 +1087,11 @@
       <c r="J14" s="1">
         <v>270765</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -996,8 +1122,11 @@
       <c r="J15" s="1">
         <v>5332</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1028,8 +1157,11 @@
       <c r="J16" s="1">
         <v>13579</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1060,8 +1192,11 @@
       <c r="J17" s="1">
         <v>7202</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1092,8 +1227,11 @@
       <c r="J18" s="1">
         <v>873.64601000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1124,8 +1262,11 @@
       <c r="J19" s="1">
         <v>59874</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -1156,8 +1297,11 @@
       <c r="J20" s="1">
         <v>21796</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1188,8 +1332,11 @@
       <c r="J21" s="1">
         <v>34704</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1220,8 +1367,11 @@
       <c r="J22" s="1">
         <v>42625</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -1252,8 +1402,11 @@
       <c r="J23" s="1">
         <v>1935</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1284,8 +1437,11 @@
       <c r="J24" s="1">
         <v>16101</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
@@ -1316,8 +1472,11 @@
       <c r="J25" s="1">
         <v>3046</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -1348,8 +1507,11 @@
       <c r="J26" s="1">
         <v>4817</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
@@ -1380,8 +1542,11 @@
       <c r="J27" s="1">
         <v>17388</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -1412,8 +1577,11 @@
       <c r="J28" s="1">
         <v>45001</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -1444,8 +1612,11 @@
       <c r="J29" s="4">
         <v>1428403</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K29" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -1476,8 +1647,11 @@
       <c r="J30" s="1">
         <v>160477</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1508,8 +1682,11 @@
       <c r="J31" s="1">
         <v>29647</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
@@ -1540,8 +1717,11 @@
       <c r="J32" s="1">
         <v>126951</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1572,8 +1752,11 @@
       <c r="J33" s="1">
         <v>135348</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1604,8 +1787,11 @@
       <c r="J34" s="1">
         <v>33627</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
@@ -1636,8 +1822,11 @@
       <c r="J35" s="1">
         <v>58110</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>17</v>
       </c>
@@ -1668,8 +1857,11 @@
       <c r="J36" s="1">
         <v>56360</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>18</v>
       </c>
@@ -1700,8 +1892,11 @@
       <c r="J37" s="1">
         <v>7054</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1732,8 +1927,11 @@
       <c r="J38" s="1">
         <v>69828</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
@@ -1764,8 +1962,11 @@
       <c r="J39" s="1">
         <v>59970</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>21</v>
       </c>
@@ -1796,8 +1997,11 @@
       <c r="J40" s="1">
         <v>118299</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
@@ -1828,8 +2032,11 @@
       <c r="J41" s="1">
         <v>284207</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>23</v>
       </c>
@@ -1860,8 +2067,11 @@
       <c r="J42" s="1">
         <v>4972</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>24</v>
       </c>
@@ -1892,8 +2102,11 @@
       <c r="J43" s="1">
         <v>14789</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>25</v>
       </c>
@@ -1924,8 +2137,11 @@
       <c r="J44" s="1">
         <v>7204</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>26</v>
       </c>
@@ -1956,8 +2172,11 @@
       <c r="J45" s="1">
         <v>932.47335999999996</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>27</v>
       </c>
@@ -1988,8 +2207,11 @@
       <c r="J46" s="1">
         <v>61116</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>28</v>
       </c>
@@ -2020,8 +2242,11 @@
       <c r="J47" s="1">
         <v>23003</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>29</v>
       </c>
@@ -2052,8 +2277,11 @@
       <c r="J48" s="1">
         <v>36193</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
@@ -2084,8 +2312,11 @@
       <c r="J49" s="1">
         <v>44096</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
@@ -2116,8 +2347,11 @@
       <c r="J50" s="1">
         <v>2375</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>32</v>
       </c>
@@ -2148,8 +2382,11 @@
       <c r="J51" s="1">
         <v>17965</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>33</v>
       </c>
@@ -2180,8 +2417,11 @@
       <c r="J52" s="1">
         <v>3616</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
@@ -2212,8 +2452,11 @@
       <c r="J53" s="1">
         <v>4914</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>35</v>
       </c>
@@ -2244,8 +2487,11 @@
       <c r="J54" s="1">
         <v>18974</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>36</v>
       </c>
@@ -2276,8 +2522,11 @@
       <c r="J55" s="1">
         <v>48377</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>10</v>
       </c>
@@ -2308,8 +2557,11 @@
       <c r="J56" s="4">
         <v>1497521</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K56" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>11</v>
       </c>
@@ -2340,8 +2592,11 @@
       <c r="J57" s="1">
         <v>169929</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>12</v>
       </c>
@@ -2372,8 +2627,11 @@
       <c r="J58" s="1">
         <v>31712</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>13</v>
       </c>
@@ -2404,8 +2662,11 @@
       <c r="J59" s="1">
         <v>133642</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>14</v>
       </c>
@@ -2436,8 +2697,11 @@
       <c r="J60" s="1">
         <v>142122</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>15</v>
       </c>
@@ -2468,8 +2732,11 @@
       <c r="J61" s="1">
         <v>35969</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>16</v>
       </c>
@@ -2500,8 +2767,11 @@
       <c r="J62" s="1">
         <v>60209</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>17</v>
       </c>
@@ -2532,8 +2802,11 @@
       <c r="J63" s="1">
         <v>58329</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>18</v>
       </c>
@@ -2564,8 +2837,11 @@
       <c r="J64" s="1">
         <v>7556</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K64" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>19</v>
       </c>
@@ -2596,8 +2872,11 @@
       <c r="J65" s="1">
         <v>72719</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K65" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -2628,8 +2907,11 @@
       <c r="J66" s="1">
         <v>59710</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>21</v>
       </c>
@@ -2660,8 +2942,11 @@
       <c r="J67" s="1">
         <v>125195</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K67" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>22</v>
       </c>
@@ -2692,8 +2977,11 @@
       <c r="J68" s="1">
         <v>296724</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K68" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>23</v>
       </c>
@@ -2724,8 +3012,11 @@
       <c r="J69" s="1">
         <v>5230</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K69" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>24</v>
       </c>
@@ -2756,8 +3047,11 @@
       <c r="J70" s="1">
         <v>14940</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K70" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>25</v>
       </c>
@@ -2788,8 +3082,11 @@
       <c r="J71" s="1">
         <v>8209</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K71" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>26</v>
       </c>
@@ -2820,8 +3117,11 @@
       <c r="J72" s="1">
         <v>828.56652999999994</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K72" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>27</v>
       </c>
@@ -2852,8 +3152,11 @@
       <c r="J73" s="1">
         <v>62978</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K73" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>28</v>
       </c>
@@ -2884,8 +3187,11 @@
       <c r="J74" s="1">
         <v>24380</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>29</v>
       </c>
@@ -2916,8 +3222,11 @@
       <c r="J75" s="1">
         <v>38569</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K75" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -2948,8 +3257,11 @@
       <c r="J76" s="1">
         <v>50151</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K76" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>31</v>
       </c>
@@ -2980,8 +3292,11 @@
       <c r="J77" s="1">
         <v>2556</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K77" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>32</v>
       </c>
@@ -3012,8 +3327,11 @@
       <c r="J78" s="1">
         <v>17867</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K78" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>33</v>
       </c>
@@ -3044,8 +3362,11 @@
       <c r="J79" s="1">
         <v>3250</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K79" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -3076,8 +3397,11 @@
       <c r="J80" s="1">
         <v>4758</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K80" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>35</v>
       </c>
@@ -3108,8 +3432,11 @@
       <c r="J81" s="1">
         <v>19690</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K81" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>36</v>
       </c>
@@ -3140,8 +3467,11 @@
       <c r="J82" s="1">
         <v>50296</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>10</v>
       </c>
@@ -3172,8 +3502,11 @@
       <c r="J83" s="4">
         <v>1572027</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K83" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>11</v>
       </c>
@@ -3204,8 +3537,11 @@
       <c r="J84" s="1">
         <v>175774</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>12</v>
       </c>
@@ -3236,8 +3572,11 @@
       <c r="J85" s="1">
         <v>34352</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K85" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>13</v>
       </c>
@@ -3268,8 +3607,11 @@
       <c r="J86" s="1">
         <v>134063</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K86" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>14</v>
       </c>
@@ -3300,8 +3642,11 @@
       <c r="J87" s="1">
         <v>151665</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K87" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>15</v>
       </c>
@@ -3332,8 +3677,11 @@
       <c r="J88" s="1">
         <v>38365</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K88" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>16</v>
       </c>
@@ -3364,8 +3712,11 @@
       <c r="J89" s="1">
         <v>62660</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K89" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>17</v>
       </c>
@@ -3396,8 +3747,11 @@
       <c r="J90" s="1">
         <v>61095</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K90" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>18</v>
       </c>
@@ -3428,8 +3782,11 @@
       <c r="J91" s="1">
         <v>7432</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K91" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>19</v>
       </c>
@@ -3460,8 +3817,11 @@
       <c r="J92" s="1">
         <v>73591</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K92" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>20</v>
       </c>
@@ -3492,8 +3852,11 @@
       <c r="J93" s="1">
         <v>65610</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K93" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>21</v>
       </c>
@@ -3524,8 +3887,11 @@
       <c r="J94" s="1">
         <v>133778</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K94" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>22</v>
       </c>
@@ -3556,8 +3922,11 @@
       <c r="J95" s="1">
         <v>310429</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K95" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>23</v>
       </c>
@@ -3588,8 +3957,11 @@
       <c r="J96" s="1">
         <v>6306</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>24</v>
       </c>
@@ -3620,8 +3992,11 @@
       <c r="J97" s="1">
         <v>15378</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K97" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>25</v>
       </c>
@@ -3652,8 +4027,11 @@
       <c r="J98" s="1">
         <v>7755</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K98" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>26</v>
       </c>
@@ -3684,8 +4062,11 @@
       <c r="J99" s="1">
         <v>1099</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K99" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>27</v>
       </c>
@@ -3716,8 +4097,11 @@
       <c r="J100" s="1">
         <v>67350</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K100" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>28</v>
       </c>
@@ -3748,8 +4132,11 @@
       <c r="J101" s="1">
         <v>26377</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K101" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>29</v>
       </c>
@@ -3780,8 +4167,11 @@
       <c r="J102" s="1">
         <v>41488</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K102" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>30</v>
       </c>
@@ -3812,8 +4202,11 @@
       <c r="J103" s="1">
         <v>51567</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K103" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>31</v>
       </c>
@@ -3844,8 +4237,11 @@
       <c r="J104" s="1">
         <v>2951</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K104" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>32</v>
       </c>
@@ -3876,8 +4272,11 @@
       <c r="J105" s="1">
         <v>21037</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K105" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>33</v>
       </c>
@@ -3908,8 +4307,11 @@
       <c r="J106" s="1">
         <v>3680</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K106" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>34</v>
       </c>
@@ -3940,8 +4342,11 @@
       <c r="J107" s="1">
         <v>6095</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K107" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>35</v>
       </c>
@@ -3972,8 +4377,11 @@
       <c r="J108" s="1">
         <v>20420</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K108" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>36</v>
       </c>
@@ -4004,8 +4412,11 @@
       <c r="J109" s="1">
         <v>51710</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K109" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>10</v>
       </c>
@@ -4036,8 +4447,11 @@
       <c r="J110" s="4">
         <v>1653568</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K110" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>11</v>
       </c>
@@ -4068,8 +4482,11 @@
       <c r="J111" s="1">
         <v>190691</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K111" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>12</v>
       </c>
@@ -4100,8 +4517,11 @@
       <c r="J112" s="1">
         <v>35745</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K112" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>13</v>
       </c>
@@ -4132,8 +4552,11 @@
       <c r="J113" s="1">
         <v>143699</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K113" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>14</v>
       </c>
@@ -4164,8 +4587,11 @@
       <c r="J114" s="1">
         <v>158270</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K114" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>15</v>
       </c>
@@ -4196,8 +4622,11 @@
       <c r="J115" s="1">
         <v>41158</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K115" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>16</v>
       </c>
@@ -4228,8 +4657,11 @@
       <c r="J116" s="1">
         <v>64566</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K116" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>17</v>
       </c>
@@ -4260,8 +4692,11 @@
       <c r="J117" s="1">
         <v>62261</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K117" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>18</v>
       </c>
@@ -4292,8 +4727,11 @@
       <c r="J118" s="1">
         <v>8732</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K118" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>19</v>
       </c>
@@ -4324,8 +4762,11 @@
       <c r="J119" s="1">
         <v>74825</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K119" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>20</v>
       </c>
@@ -4356,8 +4797,11 @@
       <c r="J120" s="1">
         <v>68312</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K120" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>21</v>
       </c>
@@ -4388,8 +4832,11 @@
       <c r="J121" s="1">
         <v>143428</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K121" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>22</v>
       </c>
@@ -4420,8 +4867,11 @@
       <c r="J122" s="1">
         <v>328713</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K122" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>23</v>
       </c>
@@ -4452,8 +4902,11 @@
       <c r="J123" s="1">
         <v>5957</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K123" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>24</v>
       </c>
@@ -4484,8 +4937,11 @@
       <c r="J124" s="1">
         <v>15552</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K124" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>25</v>
       </c>
@@ -4516,8 +4972,11 @@
       <c r="J125" s="1">
         <v>8423</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K125" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>26</v>
       </c>
@@ -4548,8 +5007,11 @@
       <c r="J126" s="1">
         <v>1088</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K126" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>27</v>
       </c>
@@ -4580,8 +5042,11 @@
       <c r="J127" s="1">
         <v>71183</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K127" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>28</v>
       </c>
@@ -4612,8 +5077,11 @@
       <c r="J128" s="1">
         <v>24324</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K128" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>29</v>
       </c>
@@ -4644,8 +5112,11 @@
       <c r="J129" s="1">
         <v>42803</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K129" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>30</v>
       </c>
@@ -4676,8 +5147,11 @@
       <c r="J130" s="1">
         <v>54229</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K130" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>31</v>
       </c>
@@ -4708,8 +5182,11 @@
       <c r="J131" s="1">
         <v>2917</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K131" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>32</v>
       </c>
@@ -4740,8 +5217,11 @@
       <c r="J132" s="1">
         <v>22012</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K132" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>33</v>
       </c>
@@ -4772,8 +5252,11 @@
       <c r="J133" s="1">
         <v>3886</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K133" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>34</v>
       </c>
@@ -4804,8 +5287,11 @@
       <c r="J134" s="1">
         <v>5630</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K134" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>35</v>
       </c>
@@ -4836,8 +5322,11 @@
       <c r="J135" s="1">
         <v>22104</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K135" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>36</v>
       </c>
@@ -4868,8 +5357,11 @@
       <c r="J136" s="1">
         <v>53057</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K136" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>10</v>
       </c>
@@ -4900,8 +5392,11 @@
       <c r="J137" s="4">
         <v>1740916.5161851901</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K137" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>11</v>
       </c>
@@ -4932,8 +5427,11 @@
       <c r="J138" s="1">
         <v>198852.07086324101</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K138" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>12</v>
       </c>
@@ -4964,8 +5462,11 @@
       <c r="J139" s="1">
         <v>39286.471767380499</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K139" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>13</v>
       </c>
@@ -4996,8 +5497,11 @@
       <c r="J140" s="1">
         <v>151693.66559743701</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K140" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>14</v>
       </c>
@@ -5028,8 +5532,11 @@
       <c r="J141" s="1">
         <v>168953.15633999801</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K141" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>15</v>
       </c>
@@ -5060,8 +5567,11 @@
       <c r="J142" s="1">
         <v>42616.413113732102</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K142" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>16</v>
       </c>
@@ -5092,8 +5602,11 @@
       <c r="J143" s="1">
         <v>69771.327424785399</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K143" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>17</v>
       </c>
@@ -5124,8 +5637,11 @@
       <c r="J144" s="1">
         <v>65447.699883351503</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K144" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>18</v>
       </c>
@@ -5156,8 +5672,11 @@
       <c r="J145" s="1">
         <v>8807.0101925609997</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K145" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>19</v>
       </c>
@@ -5188,8 +5707,11 @@
       <c r="J146" s="1">
         <v>77321.307175027701</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K146" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
         <v>20</v>
       </c>
@@ -5220,8 +5742,11 @@
       <c r="J147" s="1">
         <v>69684.096558527104</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K147" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>21</v>
       </c>
@@ -5252,8 +5777,11 @@
       <c r="J148" s="1">
         <v>145897.37864216801</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K148" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>22</v>
       </c>
@@ -5284,8 +5812,11 @@
       <c r="J149" s="1">
         <v>340852.10092930502</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K149" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
         <v>23</v>
       </c>
@@ -5316,8 +5847,11 @@
       <c r="J150" s="1">
         <v>7168.69617519844</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K150" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>24</v>
       </c>
@@ -5348,8 +5882,11 @@
       <c r="J151" s="1">
         <v>17082.587119284599</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K151" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
         <v>25</v>
       </c>
@@ -5380,8 +5917,11 @@
       <c r="J152" s="1">
         <v>9634.0595574468407</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K152" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
         <v>26</v>
       </c>
@@ -5412,8 +5952,11 @@
       <c r="J153" s="1">
         <v>1189.3325193016699</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K153" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
         <v>27</v>
       </c>
@@ -5444,8 +5987,11 @@
       <c r="J154" s="1">
         <v>74587.011503593603</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K154" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
         <v>28</v>
       </c>
@@ -5476,8 +6022,11 @@
       <c r="J155" s="1">
         <v>27659.074949431601</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K155" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
         <v>29</v>
       </c>
@@ -5508,8 +6057,11 @@
       <c r="J156" s="1">
         <v>48175.351028462297</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K156" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
         <v>30</v>
       </c>
@@ -5540,8 +6092,11 @@
       <c r="J157" s="1">
         <v>55887.248586481997</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K157" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
         <v>31</v>
       </c>
@@ -5572,8 +6127,11 @@
       <c r="J158" s="1">
         <v>2912.1074638851901</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K158" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
         <v>32</v>
       </c>
@@ -5604,8 +6162,11 @@
       <c r="J159" s="1">
         <v>24893.387150737399</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K159" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
         <v>33</v>
       </c>
@@ -5636,8 +6197,11 @@
       <c r="J160" s="1">
         <v>4220.1649579956002</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K160" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>34</v>
       </c>
@@ -5668,8 +6232,11 @@
       <c r="J161" s="1">
         <v>6304.4066194142697</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K161" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>35</v>
       </c>
@@ -5700,8 +6267,11 @@
       <c r="J162" s="1">
         <v>22942.093096056102</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K162" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>36</v>
       </c>
@@ -5731,6 +6301,9 @@
       </c>
       <c r="J163" s="1">
         <v>59078.2969703821</v>
+      </c>
+      <c r="K163" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>